<commit_message>
mise à jour de la feuille de temps
</commit_message>
<xml_diff>
--- a/Document/Feuille de temps_v1.6.xlsx
+++ b/Document/Feuille de temps_v1.6.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>insertion bd</t>
+  </si>
+  <si>
+    <t>Page d'accueil</t>
+  </si>
+  <si>
+    <t>Serveur MySQL</t>
   </si>
 </sst>
 </file>
@@ -2690,7 +2696,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,7 +2752,7 @@
         <v>0.75</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2763,7 +2769,7 @@
         <v>0.75</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2780,7 +2786,7 @@
         <v>0.75</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2797,7 +2803,7 @@
         <v>0.75</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>